<commit_message>
first draft for new payment
</commit_message>
<xml_diff>
--- a/Downloads/userlist.xlsx
+++ b/Downloads/userlist.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,22 +469,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Luca</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mattana</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>lmattana</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PWD00</t>
+          <t>xxx</t>
         </is>
       </c>
     </row>
@@ -497,358 +497,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Luca </t>
+          <t>John</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Zucchero</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>lzucchero</t>
+          <t>john</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>lzucchero</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Test01</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Test01</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>test01</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>password01</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Jimi</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Hendrix</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>jimi</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>jimi</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Test03</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ZeroTre</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Test03</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Test03</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>test03</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>test03</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Test04</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Test04</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>test04</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>test04</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Test05</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Test05</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>test05</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>test05</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Test06</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Test06</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>test06</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>test06</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>gig</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>gig</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>gig</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>gig</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>xxx</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>vvv</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>vvv</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>vvv</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>vvv</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>kaz</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>kaz</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>kaz</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>kaz</t>
+          <t>smith</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Print Cash Sheet - set vault
</commit_message>
<xml_diff>
--- a/Downloads/userlist.xlsx
+++ b/Downloads/userlist.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>password</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>usertype</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -487,6 +492,11 @@
           <t>xxx</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -497,22 +507,60 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>ccc</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>ccc</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>john</t>
+          <t>ccc</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>smith</t>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>cassiere</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>cassiere</t>
         </is>
       </c>
     </row>

</xml_diff>